<commit_message>
Updated D/D/1 example - Data file modified to reflect proper IAT's - WIP: quay length should still be included
</commit_message>
<xml_diff>
--- a/notebooks/data.xlsx
+++ b/notebooks/data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{616142D6-E89B-4307-B57D-23C57ED763F2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBEE03D6-AD6C-4F5C-A767-AF6FF2A2A032}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -610,7 +610,7 @@
   <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -649,10 +649,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="3">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C2" s="3">
-        <f>F2+G2</f>
+        <f t="shared" ref="C2:C32" si="0">F2+G2</f>
         <v>3</v>
       </c>
       <c r="D2" s="3">
@@ -676,10 +676,11 @@
         <v>5</v>
       </c>
       <c r="B3" s="3">
-        <v>16</v>
+        <f>D3-D2</f>
+        <v>0</v>
       </c>
       <c r="C3" s="3">
-        <f>F3+G3</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="D3" s="3">
@@ -703,10 +704,11 @@
         <v>2</v>
       </c>
       <c r="B4" s="3">
-        <v>18</v>
+        <f>D4-D3</f>
+        <v>3</v>
       </c>
       <c r="C4" s="3">
-        <f>F4+G4</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="D4" s="3">
@@ -730,10 +732,11 @@
         <v>0</v>
       </c>
       <c r="B5" s="3">
-        <v>7</v>
+        <f t="shared" ref="B5:B32" si="1">D5-D4</f>
+        <v>4</v>
       </c>
       <c r="C5" s="3">
-        <f>F5+G5</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="D5" s="3">
@@ -757,10 +760,11 @@
         <v>4</v>
       </c>
       <c r="B6" s="3">
-        <v>10</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="C6" s="3">
-        <f>F6+G6</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="D6" s="3">
@@ -784,10 +788,11 @@
         <v>1</v>
       </c>
       <c r="B7" s="3">
-        <v>30</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="C7" s="3">
-        <f>F7+G7</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="D7" s="3">
@@ -811,10 +816,11 @@
         <v>0</v>
       </c>
       <c r="B8" s="3">
-        <v>7</v>
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
       <c r="C8" s="3">
-        <f>F8+G8</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="D8" s="3">
@@ -838,10 +844,11 @@
         <v>5</v>
       </c>
       <c r="B9" s="3">
-        <v>16</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="C9" s="3">
-        <f>F9+G9</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="D9" s="3">
@@ -865,10 +872,11 @@
         <v>4</v>
       </c>
       <c r="B10" s="3">
-        <v>10</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="C10" s="3">
-        <f>F10+G10</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="D10" s="3">
@@ -892,10 +900,11 @@
         <v>0</v>
       </c>
       <c r="B11" s="3">
-        <v>7</v>
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
       <c r="C11" s="3">
-        <f>F11+G11</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="D11" s="3">
@@ -919,10 +928,11 @@
         <v>2</v>
       </c>
       <c r="B12" s="3">
-        <v>18</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="C12" s="3">
-        <f>F12+G12</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="D12" s="3">
@@ -946,10 +956,11 @@
         <v>3</v>
       </c>
       <c r="B13" s="3">
-        <v>60</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="C13" s="3">
-        <f>F13+G13</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="D13" s="3">
@@ -973,10 +984,11 @@
         <v>4</v>
       </c>
       <c r="B14" s="3">
-        <v>10</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
       <c r="C14" s="3">
-        <f>F14+G14</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="D14" s="3">
@@ -1000,10 +1012,11 @@
         <v>0</v>
       </c>
       <c r="B15" s="3">
-        <v>7</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="C15" s="3">
-        <f>F15+G15</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="D15" s="3">
@@ -1027,10 +1040,11 @@
         <v>5</v>
       </c>
       <c r="B16" s="3">
-        <v>16</v>
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
       <c r="C16" s="3">
-        <f>F16+G16</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="D16" s="3">
@@ -1054,10 +1068,11 @@
         <v>0</v>
       </c>
       <c r="B17" s="3">
-        <v>7</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="C17" s="3">
-        <f>F17+G17</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="D17" s="3">
@@ -1081,10 +1096,11 @@
         <v>4</v>
       </c>
       <c r="B18" s="3">
-        <v>10</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="C18" s="3">
-        <f>F18+G18</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="D18" s="3">
@@ -1108,10 +1124,11 @@
         <v>2</v>
       </c>
       <c r="B19" s="3">
-        <v>18</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="C19" s="3">
-        <f>F19+G19</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="D19" s="3">
@@ -1135,10 +1152,11 @@
         <v>1</v>
       </c>
       <c r="B20" s="3">
-        <v>30</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="C20" s="3">
-        <f>F20+G20</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="D20" s="3">
@@ -1162,10 +1180,11 @@
         <v>0</v>
       </c>
       <c r="B21" s="3">
-        <v>7</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="C21" s="3">
-        <f>F21+G21</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="D21" s="3">
@@ -1189,10 +1208,11 @@
         <v>4</v>
       </c>
       <c r="B22" s="3">
-        <v>10</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
       </c>
       <c r="C22" s="3">
-        <f>F22+G22</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="D22" s="3">
@@ -1216,10 +1236,11 @@
         <v>5</v>
       </c>
       <c r="B23" s="3">
-        <v>16</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="C23" s="3">
-        <f>F23+G23</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="D23" s="3">
@@ -1243,10 +1264,11 @@
         <v>0</v>
       </c>
       <c r="B24" s="3">
-        <v>7</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="C24" s="3">
-        <f>F24+G24</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="D24" s="3">
@@ -1270,10 +1292,11 @@
         <v>0</v>
       </c>
       <c r="B25" s="3">
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="C25" s="3">
-        <f>F25+G25</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="D25" s="3">
@@ -1297,10 +1320,11 @@
         <v>2</v>
       </c>
       <c r="B26" s="3">
-        <v>18</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="C26" s="3">
-        <f>F26+G26</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="D26" s="3">
@@ -1324,10 +1348,11 @@
         <v>4</v>
       </c>
       <c r="B27" s="3">
-        <v>10</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="C27" s="3">
-        <f>F27+G27</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="D27" s="3">
@@ -1351,10 +1376,11 @@
         <v>0</v>
       </c>
       <c r="B28" s="3">
-        <v>7</v>
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="C28" s="3">
-        <f>F28+G28</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="D28" s="3">
@@ -1378,10 +1404,11 @@
         <v>5</v>
       </c>
       <c r="B29" s="3">
-        <v>16</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="C29" s="3">
-        <f>F29+G29</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="D29" s="3">
@@ -1405,10 +1432,11 @@
         <v>1</v>
       </c>
       <c r="B30" s="3">
-        <v>30</v>
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="C30" s="3">
-        <f>F30+G30</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="D30" s="3">
@@ -1432,10 +1460,11 @@
         <v>3</v>
       </c>
       <c r="B31" s="3">
-        <v>60</v>
+        <f t="shared" si="1"/>
+        <v>12</v>
       </c>
       <c r="C31" s="3">
-        <f>F31+G31</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="D31" s="3">
@@ -1459,10 +1488,11 @@
         <v>3</v>
       </c>
       <c r="B32" s="3">
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="C32" s="3">
-        <f>F32+G32</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="D32" s="3">

</xml_diff>